<commit_message>
update data consumer server CapabilityStatement
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheet/data-consumer-server.xlsx
+++ b/input/resources-spreadsheet/data-consumer-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/Davinci-CDEX/input/resources-spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4865A398-D844-A048-B1BB-046A4968FF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA5666B-5BE4-A540-BC4B-DBE5D009FAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="151">
   <si>
     <t>Element</t>
   </si>
@@ -357,14 +357,6 @@
   </si>
   <si>
     <t>http://www.hl7.org/Special/committees/patientcare/index.cfm</t>
-  </si>
-  <si>
-    <t>0.2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
-1. For security considerations specific to this guide refer to the Da Vinci HRex Implementation Guide section on [Security and Privacy](http://hl7.org/fhir/us/davinci-hrex/2020Sep/security.html)
-</t>
   </si>
   <si>
     <t>HRex Task Data Request Profile</t>
@@ -446,90 +438,119 @@
     <t>!http://hl7.org/fhir/us/davinci-hrex/StructureDefinition/hrex-task-data-request</t>
   </si>
   <si>
+    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
+  </si>
+  <si>
+    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
+  </si>
+  <si>
+    <t>suppress_may_sps</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>json,xml</t>
+  </si>
+  <si>
+    <t>format_conf</t>
+  </si>
+  <si>
+    <t>SHALL,SHOULD</t>
+  </si>
+  <si>
+    <t>patchFormat</t>
+  </si>
+  <si>
+    <t>application/json-patch+json</t>
+  </si>
+  <si>
+    <t>patchFormat_conf</t>
+  </si>
+  <si>
+    <t>canonical</t>
+  </si>
+  <si>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>instantiates</t>
+  </si>
+  <si>
+    <t>include_conf</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>revinclude</t>
+  </si>
+  <si>
+    <t>revinclude_conf</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/index.html</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
     <t>This CapabilityStatement describes the expected capabilities of a Da Vinci CDex Data Consumer (often a Payer) in *Server* mode when  responding to a  Data Source  (often an EHR) or one of its proxies during a clinical data exchange.   This includes the following interactions:
-1. Responding to a query for Authorization information represented by a CommunicationRequest or ServiceRequest
-1. Responding to Subscription Notification posted to it endpoint updating the status of a Task</t>
-  </si>
-  <si>
-    <t>HL7 FHIR® US Core Implementation Guide STU3 Release 3.1.1</t>
-  </si>
-  <si>
-    <t>Da Vinci Health Record Exchange (HRex) 0.2.0 - STU R1 - 2nd ballot</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/input/</t>
-  </si>
-  <si>
-    <t>/users/ehaas/Documents/FHIR/Davinci-CDEX/output/</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|0.2.0</t>
-  </si>
-  <si>
-    <t>suppress_may_sps</t>
-  </si>
-  <si>
-    <t>format</t>
-  </si>
-  <si>
-    <t>json,xml</t>
-  </si>
-  <si>
-    <t>format_conf</t>
-  </si>
-  <si>
-    <t>SHALL,SHOULD</t>
-  </si>
-  <si>
-    <t>patchFormat</t>
-  </si>
-  <si>
-    <t>application/json-patch+json</t>
-  </si>
-  <si>
-    <t>patchFormat_conf</t>
-  </si>
-  <si>
-    <t>canonical</t>
-  </si>
-  <si>
-    <t>imports</t>
-  </si>
-  <si>
-    <t>instantiates</t>
-  </si>
-  <si>
-    <t>include_conf</t>
-  </si>
-  <si>
-    <t>include</t>
-  </si>
-  <si>
-    <t>revinclude</t>
-  </si>
-  <si>
-    <t>revinclude_conf</t>
-  </si>
-  <si>
-    <t>The  Da Vinci CDex Data Consumer  **SHALL**:
-1. Support  theTask Based Approach approaches for requesting information as defined in this Guide:
-1. Support json source formats for all Da Vinci CDex interactions.
-1. Declare a CapabilityStatement identifying  transactions and profiles supported.
-The  Da Vinci CDex Data Consumer  **SHOULD**:
+1. Responding to a query for authorization information represented by a CommunicationRequest or ServiceRequest
+1. Responding to subscription notification posted to it endpoint updating the status of a task
+1. Responding to `$submit-attachment` operation.</t>
+  </si>
+  <si>
+    <t>The  Da Vinci CDex Data Consumer **SHALL**:
+1. Support at least one of the these FHIR transaction approaches for exchanging clinical information as defined in this Guide:
+     1. Task Based Approach
+     1. Attachments
+1. Follow the guidelines for [Generating and Verifying Signed Resources](signatures.html) *if signatures are required*.
+1. Support JSON source formats for all Da Vinci CDex interactions.
+1. Declare a CapabilityStatement identifying the scenarios, transactions and profiles supported.
+The  Da Vinci CDex Data Consumer **SHOULD**:
 1. Support xml source formats for all Da Vinci CDex interactions.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/index.html</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-hrex/2020Sep/index.html</t>
+    <t>1. For general security consideration refer to the FHIR [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
+1. For security considerations specific to this guide refer to the [Security and Privacy](security.html) section.</t>
+  </si>
+  <si>
+    <t>Data Consumer Server CapabilityStatement</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/CapabilityStatement/data-consumer-server</t>
+  </si>
+  <si>
+    <t>system</t>
+  </si>
+  <si>
+    <t>submit-attachment</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/davinci-cdex/OperationDefinition/submit-attachment</t>
+  </si>
+  <si>
+    <t>If [Attachments](attachments.html) is supported, the Data Consumer Server **SHALL**  support the '$submit-attachment` operation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,18 +610,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF005C00"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -628,7 +637,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -645,27 +654,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -689,13 +683,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1032,7 +1022,7 @@
         <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1041,7 +1031,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1086,7 +1076,7 @@
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="b">
         <v>0</v>
@@ -2324,7 +2314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2347,7 +2337,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2355,7 +2345,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2371,7 +2361,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2379,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2387,7 +2377,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2395,39 +2385,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2440,7 +2430,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2455,7 +2445,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>85</v>
@@ -2466,27 +2456,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -2501,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EE0F7C-7CC8-1246-B806-09A74CA0DE20}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2518,16 +2508,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>85</v>
@@ -2537,9 +2527,21 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="17"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2551,7 +2553,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2582,25 +2584,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
@@ -2612,21 +2614,21 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
+      <c r="A4" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+      <c r="E4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G5" s="1"/>
@@ -2664,10 +2666,10 @@
   <dimension ref="A1:Y26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:Y1"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2751,49 +2753,49 @@
         <v>73</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="33" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="22:25" ht="18" x14ac:dyDescent="0.2">
@@ -2814,20 +2816,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="77.5" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" customWidth="1"/>
-    <col min="5" max="5" width="89" customWidth="1"/>
+    <col min="5" max="5" width="98.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -2844,11 +2846,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
@@ -2865,7 +2878,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:G10"/>
+      <selection pane="topRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2884,22 +2897,22 @@
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -2926,7 +2939,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>52</v>
@@ -2935,7 +2948,7 @@
         <v>52</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2948,13 +2961,13 @@
         <v>52</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>25</v>
@@ -2994,7 +3007,7 @@
         <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -3101,7 +3114,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -3111,7 +3124,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>25</v>
@@ -3119,7 +3132,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>25</v>
@@ -3127,7 +3140,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>

</xml_diff>